<commit_message>
Added LTSpice simulations for all examples and marked those that pass.
</commit_message>
<xml_diff>
--- a/OpAmp.xlsx
+++ b/OpAmp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\OpAmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D16C3A8-95B0-4B73-8E7A-68100A2E75A3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3C9D4A-A534-4A9B-9C50-5D00C82F7C00}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32835" windowHeight="15795" xr2:uid="{D6C93E9B-8E91-4E75-A6F3-2E8A3339D527}"/>
   </bookViews>
@@ -382,7 +382,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="67">
   <si>
     <t>Vinfs</t>
   </si>
@@ -519,9 +519,6 @@
     <t>Twelve Rules for Operational Amplifiers</t>
   </si>
   <si>
-    <t>Verson 1.0, 20180609, Marten Agren</t>
-  </si>
-  <si>
     <t>Transfer function:</t>
   </si>
   <si>
@@ -574,6 +571,18 @@
   </si>
   <si>
     <t>example</t>
+  </si>
+  <si>
+    <t>verified</t>
+  </si>
+  <si>
+    <t>mpbne</t>
+  </si>
+  <si>
+    <t>unverified</t>
+  </si>
+  <si>
+    <t>Verson 1.1, 20180609, Marten Agren</t>
   </si>
 </sst>
 </file>
@@ -587,7 +596,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +687,13 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -785,7 +801,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -886,6 +902,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1060,15 +1084,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>228251</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>656771</xdr:colOff>
+      <xdr:colOff>675821</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>18823</xdr:rowOff>
+      <xdr:rowOff>56922</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1091,8 +1115,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12315825" y="1390650"/>
-          <a:ext cx="3628571" cy="1819048"/>
+          <a:off x="5657501" y="923924"/>
+          <a:ext cx="3495570" cy="1752373"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1143,11 +1167,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>41606</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3714749" cy="1933333"/>
+    <xdr:ext cx="3543299" cy="1844102"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="Picture 8">
@@ -1169,8 +1193,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13670616" y="6692153"/>
-          <a:ext cx="3714749" cy="1933333"/>
+          <a:off x="17640300" y="946481"/>
+          <a:ext cx="3543299" cy="1844102"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1343,14 +1367,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>235323</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:colOff>225798</xdr:colOff>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>168088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>538718</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:colOff>529193</xdr:colOff>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1381,7 +1405,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5838264" y="6745941"/>
+          <a:off x="5655048" y="12407713"/>
           <a:ext cx="3351395" cy="1467971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2066,29 +2090,45 @@
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>50</v>
+      </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="9"/>
+      <c r="M4" s="47" t="s">
+        <v>65</v>
+      </c>
       <c r="N4" s="8"/>
-      <c r="O4" s="7"/>
+      <c r="O4" s="48" t="s">
+        <v>51</v>
+      </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
-      <c r="S4" s="9"/>
-      <c r="U4" s="7"/>
+      <c r="S4" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" s="48" t="s">
+        <v>55</v>
+      </c>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
-      <c r="Y4" s="9"/>
-      <c r="AA4" s="7"/>
+      <c r="Y4" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA4" s="48" t="s">
+        <v>64</v>
+      </c>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
-      <c r="AE4" s="9"/>
+      <c r="AE4" s="47" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="I5" s="7"/>
@@ -2138,10 +2178,10 @@
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="8"/>
@@ -2166,6 +2206,7 @@
       <c r="AE7" s="9"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="G8" s="4"/>
       <c r="I8" s="7"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -2190,7 +2231,7 @@
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="8"/>
@@ -2239,10 +2280,10 @@
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
@@ -2361,7 +2402,7 @@
       </c>
       <c r="C15" s="39">
         <f>VLOOKUP(C11,examples,4,)</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -2418,7 +2459,7 @@
       </c>
       <c r="C16" s="39">
         <f>VLOOKUP(C11,examples,5,)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -2515,7 +2556,7 @@
       </c>
       <c r="C18" s="34">
         <f>(C16-C15)/(C14-C13)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -2526,11 +2567,11 @@
       </c>
       <c r="K18" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
-      </c>
-      <c r="L18" s="10">
+        <v>3</v>
+      </c>
+      <c r="L18" s="10" t="e">
         <f>L21*K16+L22</f>
-        <v>-10.132231404958677</v>
+        <v>#N/A</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="8"/>
@@ -2540,7 +2581,7 @@
       </c>
       <c r="Q18" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R18" s="10" t="e">
         <f>R21*Q16+R22</f>
@@ -2553,7 +2594,7 @@
       </c>
       <c r="W18" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="X18" s="10" t="e">
         <f>X21*W16+X22</f>
@@ -2566,11 +2607,11 @@
       </c>
       <c r="AC18" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
-      </c>
-      <c r="AD18" s="10">
+        <v>3</v>
+      </c>
+      <c r="AD18" s="10" t="e">
         <f>AD21*AC16+AD22</f>
-        <v>-10.545454545454547</v>
+        <v>#N/A</v>
       </c>
       <c r="AE18" s="9"/>
     </row>
@@ -2580,7 +2621,7 @@
       </c>
       <c r="C19" s="34">
         <f>C15-C18*C13</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>39</v>
@@ -2592,11 +2633,11 @@
       </c>
       <c r="K19" s="21">
         <f>Voutfs</f>
-        <v>1</v>
-      </c>
-      <c r="L19" s="10">
+        <v>-1</v>
+      </c>
+      <c r="L19" s="10" t="e">
         <f>L21*K17+L22</f>
-        <v>0.13223140495867813</v>
+        <v>#N/A</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="8"/>
@@ -2606,7 +2647,7 @@
       </c>
       <c r="Q19" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R19" s="10" t="e">
         <f>R21*Q17+R22</f>
@@ -2619,7 +2660,7 @@
       </c>
       <c r="W19" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X19" s="10" t="e">
         <f>X21*W17+X22</f>
@@ -2632,11 +2673,11 @@
       </c>
       <c r="AC19" s="21">
         <f>Voutfs</f>
-        <v>1</v>
-      </c>
-      <c r="AD19" s="10">
+        <v>-1</v>
+      </c>
+      <c r="AD19" s="10" t="e">
         <f>AD21*AC17+AD22</f>
-        <v>0.54545454545454586</v>
+        <v>#N/A</v>
       </c>
       <c r="AE19" s="9"/>
     </row>
@@ -2677,7 +2718,7 @@
     </row>
     <row r="21" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="8" t="s">
@@ -2685,11 +2726,11 @@
       </c>
       <c r="K21" s="10">
         <f>(K19-K18)/(K17-K16)</f>
-        <v>2</v>
-      </c>
-      <c r="L21" s="29">
+        <v>-2</v>
+      </c>
+      <c r="L21" s="29" t="e">
         <f>K23*(1+L25/L28)</f>
-        <v>5.1322314049586772</v>
+        <v>#N/A</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="8"/>
@@ -2699,7 +2740,7 @@
       </c>
       <c r="Q21" s="10">
         <f>(Q19-Q18)/(Q17-Q16)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R21" s="29" t="e">
         <f>Q23*IF(ISNUMBER(#REF!),(#REF!*R24/R25+#REF!)/(#REF!+#REF!),R24/R25+1)</f>
@@ -2712,7 +2753,7 @@
       </c>
       <c r="W21" s="10">
         <f>(W19-W18)/(W17-W16)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="X21" s="29" t="e">
         <f>W23*IF(ISNUMBER(X25),(X25*X26/X27+X25)/(X24+X25),X26/X27+1)</f>
@@ -2725,11 +2766,11 @@
       </c>
       <c r="AC21" s="10">
         <f>(AC19-AC18)/(AC17-AC16)</f>
-        <v>2</v>
-      </c>
-      <c r="AD21" s="29">
+        <v>-2</v>
+      </c>
+      <c r="AD21" s="29" t="e">
         <f>AC23*(1+AD26/AD27)</f>
-        <v>5.5454545454545459</v>
+        <v>#N/A</v>
       </c>
       <c r="AE21" s="9"/>
     </row>
@@ -2740,11 +2781,11 @@
       </c>
       <c r="K22" s="10">
         <f>K18-K21*K16</f>
-        <v>-1</v>
-      </c>
-      <c r="L22" s="29">
+        <v>1</v>
+      </c>
+      <c r="L22" s="29" t="e">
         <f>-K23*L29*(L27+L25)/L27</f>
-        <v>-4.9999999999999991</v>
+        <v>#N/A</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="8"/>
@@ -2754,7 +2795,7 @@
       </c>
       <c r="Q22" s="10">
         <f>Q18-Q21*Q16</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R22" s="29" t="e">
         <f>Q23*0</f>
@@ -2767,7 +2808,7 @@
       </c>
       <c r="W22" s="10">
         <f>W18-W21*W16</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X22" s="29" t="e">
         <f>W23*IF(ISNUMBER(X25),W20*X24*X21/X25,0)</f>
@@ -2780,11 +2821,11 @@
       </c>
       <c r="AC22" s="10">
         <f>AC18-AC21*AC16</f>
-        <v>-1</v>
-      </c>
-      <c r="AD22" s="29">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="29" t="e">
         <f>-AD21*AD28</f>
-        <v>-5</v>
+        <v>#N/A</v>
       </c>
       <c r="AE22" s="9"/>
     </row>
@@ -2802,9 +2843,9 @@
       <c r="J23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="12" t="e">
         <f>IF(AND(K21&gt;1,K22&lt;0),1,NA())</f>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="L23" s="12"/>
       <c r="M23" s="9"/>
@@ -2833,9 +2874,9 @@
       <c r="AB23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="12">
+      <c r="AC23" s="12" t="e">
         <f>IF(AND(AC21&gt;1,AC22&lt;0),1,NA())</f>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="AD23" s="12"/>
       <c r="AE23" s="9"/>
@@ -2849,12 +2890,13 @@
       <c r="J24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="24" t="e">
         <f>K23*K26*(K20-K29)/K29</f>
-        <v>9555.5555555555566</v>
-      </c>
-      <c r="L24" s="14">
-        <v>1000</v>
+        <v>#N/A</v>
+      </c>
+      <c r="L24" s="14" t="e">
+        <f>K24</f>
+        <v>#N/A</v>
       </c>
       <c r="M24" s="9"/>
       <c r="N24" s="8"/>
@@ -2901,11 +2943,11 @@
         <v>9</v>
       </c>
       <c r="K25" s="14">
-        <v>10000</v>
+        <v>22000</v>
       </c>
       <c r="L25" s="24">
         <f>K25</f>
-        <v>10000</v>
+        <v>22000</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="8"/>
@@ -2938,9 +2980,9 @@
       <c r="AB25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AC25" s="16">
+      <c r="AC25" s="16" t="e">
         <f>AC23*AC28*AC24/(AC20-AC28)</f>
-        <v>1111.1111111111111</v>
+        <v>#N/A</v>
       </c>
       <c r="AD25" s="14">
         <v>2200</v>
@@ -2952,12 +2994,13 @@
       <c r="J26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="25" t="e">
         <f>K28/10</f>
-        <v>1000</v>
-      </c>
-      <c r="L26" s="14">
-        <v>220</v>
+        <v>#N/A</v>
+      </c>
+      <c r="L26" s="14" t="e">
+        <f>K26</f>
+        <v>#N/A</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="8"/>
@@ -2995,12 +3038,13 @@
       <c r="J27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K27" s="16">
+      <c r="K27" s="16" t="e">
         <f>K28-K26</f>
-        <v>9000</v>
-      </c>
-      <c r="L27" s="14">
-        <v>2200</v>
+        <v>#N/A</v>
+      </c>
+      <c r="L27" s="14" t="e">
+        <f>K27</f>
+        <v>#N/A</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="8"/>
@@ -3026,9 +3070,9 @@
       <c r="AB27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AC27" s="16">
+      <c r="AC27" s="16" t="e">
         <f>AC23*AC26/(AC21-1)</f>
-        <v>10000</v>
+        <v>#N/A</v>
       </c>
       <c r="AD27" s="14">
         <v>2200</v>
@@ -3040,13 +3084,13 @@
       <c r="J28" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K28" s="26">
+      <c r="K28" s="26" t="e">
         <f>K23*K25/(K21-1)</f>
-        <v>10000</v>
-      </c>
-      <c r="L28" s="26">
+        <v>#N/A</v>
+      </c>
+      <c r="L28" s="26" t="e">
         <f>L27+L26</f>
-        <v>2420</v>
+        <v>#N/A</v>
       </c>
       <c r="M28" s="9"/>
       <c r="N28" s="8"/>
@@ -3064,9 +3108,9 @@
       <c r="AB28" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AC28" s="30">
+      <c r="AC28" s="30" t="e">
         <f>AC23*ABS(AC22)/AC21</f>
-        <v>0.5</v>
+        <v>#N/A</v>
       </c>
       <c r="AD28" s="30">
         <f>AC20/(1+AD24/AD25)</f>
@@ -3079,13 +3123,13 @@
       <c r="J29" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="30">
+      <c r="K29" s="30" t="e">
         <f>K23*ABS(K22)*K27/(K27+K25)</f>
-        <v>0.47368421052631576</v>
-      </c>
-      <c r="L29" s="30">
+        <v>#N/A</v>
+      </c>
+      <c r="L29" s="30" t="e">
         <f>K20/(1+L24/L26)</f>
-        <v>0.90163934426229497</v>
+        <v>#N/A</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="8"/>
@@ -3154,7 +3198,7 @@
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>1</v>
@@ -3168,25 +3212,37 @@
       <c r="F33" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="48" t="s">
+        <v>52</v>
+      </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
-      <c r="M33" s="9"/>
-      <c r="O33" s="7"/>
+      <c r="M33" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="O33" s="48" t="s">
+        <v>53</v>
+      </c>
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
-      <c r="S33" s="9"/>
-      <c r="U33" s="7"/>
+      <c r="S33" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="U33" s="48" t="s">
+        <v>54</v>
+      </c>
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
       <c r="X33" s="8"/>
-      <c r="Y33" s="9"/>
+      <c r="Y33" s="46" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="40">
         <v>-1</v>
@@ -3218,7 +3274,7 @@
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="40">
         <v>-1</v>
@@ -3250,7 +3306,7 @@
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="40">
         <v>-1</v>
@@ -3282,7 +3338,7 @@
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="40">
         <v>-1</v>
@@ -3314,7 +3370,7 @@
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="40">
         <v>-1</v>
@@ -3346,7 +3402,7 @@
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="40">
         <v>-1</v>
@@ -3378,7 +3434,7 @@
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="40">
         <v>-1</v>
@@ -3410,7 +3466,7 @@
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="40">
         <v>-1</v>
@@ -3442,7 +3498,7 @@
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="40">
         <v>-1</v>
@@ -3474,7 +3530,7 @@
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" s="40">
         <v>-1</v>
@@ -3506,7 +3562,7 @@
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="40">
         <v>-1</v>
@@ -3556,7 +3612,7 @@
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" s="40">
         <v>-1</v>
@@ -3640,7 +3696,7 @@
       </c>
       <c r="K47" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="L47" s="10" t="e">
         <f>L50*K45+L51</f>
@@ -3653,7 +3709,7 @@
       </c>
       <c r="Q47" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R47" s="10" t="e">
         <f>R50*Q45+R51</f>
@@ -3666,7 +3722,7 @@
       </c>
       <c r="W47" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="X47" s="10" t="e">
         <f>X50*W45+X51</f>
@@ -3681,7 +3737,7 @@
       </c>
       <c r="K48" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L48" s="10" t="e">
         <f>L50*K46+L51</f>
@@ -3694,7 +3750,7 @@
       </c>
       <c r="Q48" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R48" s="10" t="e">
         <f>R50*Q46+R51</f>
@@ -3707,7 +3763,7 @@
       </c>
       <c r="W48" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X48" s="10" t="e">
         <f>X50*W46+X51</f>
@@ -3747,7 +3803,7 @@
       </c>
       <c r="K50" s="10">
         <f>(K48-K47)/(K46-K45)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="L50" s="10" t="e">
         <f>apbn*L54/(L53+L54)*(1+L55/L56)</f>
@@ -3760,7 +3816,7 @@
       </c>
       <c r="Q50" s="10">
         <f>(Q48-Q47)/(Q46-Q45)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R50" s="10" t="e">
         <f>apbz*R54/(R53+R54)</f>
@@ -3773,7 +3829,7 @@
       </c>
       <c r="W50" s="10">
         <f>(W48-W47)/(W46-W45)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="X50" s="23" t="e">
         <f>(apbp/X53)/(1/X53+1/X54+1/X55)</f>
@@ -3789,7 +3845,7 @@
       </c>
       <c r="K51" s="10">
         <f>K47-K50*K45</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L51" s="10" t="e">
         <f>-apbn*K49*L55/L56</f>
@@ -3802,7 +3858,7 @@
       </c>
       <c r="Q51" s="10">
         <f>Q47-Q50*Q45</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R51" s="10" t="e">
         <f>Q52*0</f>
@@ -3815,7 +3871,7 @@
       </c>
       <c r="W51" s="10">
         <f>W47-W50*W45</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X51" s="23" t="e">
         <f>apbp*(W49/X55)/(1/X53+1/X54+1/X55)</f>
@@ -3941,11 +3997,11 @@
         <v>9</v>
       </c>
       <c r="K55" s="14">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="L55" s="24">
         <f>K55</f>
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="M55" s="9"/>
       <c r="O55" s="7"/>
@@ -4068,22 +4124,34 @@
       <c r="Y61" s="44"/>
     </row>
     <row r="62" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="I62" s="7"/>
+      <c r="I62" s="48" t="s">
+        <v>56</v>
+      </c>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
-      <c r="M62" s="9"/>
+      <c r="M62" s="46" t="s">
+        <v>63</v>
+      </c>
       <c r="N62" s="8"/>
-      <c r="O62" s="7"/>
+      <c r="O62" s="48" t="s">
+        <v>57</v>
+      </c>
       <c r="P62" s="8"/>
       <c r="Q62" s="8"/>
       <c r="R62" s="8"/>
-      <c r="S62" s="9"/>
-      <c r="U62" s="7"/>
+      <c r="S62" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="U62" s="48" t="s">
+        <v>58</v>
+      </c>
       <c r="V62" s="8"/>
       <c r="W62" s="8"/>
       <c r="X62" s="8"/>
-      <c r="Y62" s="9"/>
+      <c r="Y62" s="46" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="63" spans="3:25" x14ac:dyDescent="0.25">
       <c r="I63" s="7"/>
@@ -4374,7 +4442,7 @@
       </c>
       <c r="K76" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="L76" s="10" t="e">
         <f>L79*K74+L80</f>
@@ -4388,7 +4456,7 @@
       </c>
       <c r="Q76" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R76" s="10" t="e">
         <f>R79*Q74+R80</f>
@@ -4401,7 +4469,7 @@
       </c>
       <c r="W76" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="X76" s="10" t="e">
         <f>X79*W74+X80</f>
@@ -4416,7 +4484,7 @@
       </c>
       <c r="K77" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L77" s="10" t="e">
         <f>L79*K75+L80</f>
@@ -4430,7 +4498,7 @@
       </c>
       <c r="Q77" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R77" s="10" t="e">
         <f>R79*Q75+R80</f>
@@ -4443,7 +4511,7 @@
       </c>
       <c r="W77" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X77" s="10" t="e">
         <f>X79*W75+X80</f>
@@ -4484,7 +4552,7 @@
       </c>
       <c r="K79" s="10">
         <f>(K77-K76)/(K75-K74)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="L79" s="29" t="e">
         <f>-apbn*IF(ISNUMBER(L85),L82*L85/(L84*(L84+2*L85)),1)</f>
@@ -4498,7 +4566,7 @@
       </c>
       <c r="Q79" s="10">
         <f>(Q77-Q76)/(Q75-Q74)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R79" s="29" t="e">
         <f>-apbz*R82*R84/(R83*(R83+2*R84))</f>
@@ -4511,10 +4579,10 @@
       </c>
       <c r="W79" s="10">
         <f>(W77-W76)/(W75-W74)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="X79" s="29" t="e">
-        <f>-apbp*X82*X84/(X83*(X83+2*X84))</f>
+        <f>-anbp*X82*X84/(X83*(X83+2*X84))</f>
         <v>#N/A</v>
       </c>
       <c r="Y79" s="9"/>
@@ -4526,7 +4594,7 @@
       </c>
       <c r="K80" s="10">
         <f>K76-K79*K74</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L80" s="10" t="e">
         <f>-K81*K78*L82/L83</f>
@@ -4540,7 +4608,7 @@
       </c>
       <c r="Q80" s="10">
         <f>Q76-Q79*Q74</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R80" s="29" t="e">
         <f>Q81*0</f>
@@ -4553,10 +4621,10 @@
       </c>
       <c r="W80" s="10">
         <f>W76-W79*W74</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X80" s="29" t="e">
-        <f>apbp*W78*(X86/(X85+X86))*(1+X82/(X83+X87))</f>
+        <f>anbp*W78*(X86/(X85+X86))*(1+X82/(X83+X87))</f>
         <v>#N/A</v>
       </c>
       <c r="Y80" s="9"/>
@@ -4600,11 +4668,11 @@
         <v>9</v>
       </c>
       <c r="K82" s="14">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="L82" s="24">
         <f>K82</f>
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="M82" s="9"/>
       <c r="N82" s="8"/>
@@ -4613,11 +4681,11 @@
         <v>9</v>
       </c>
       <c r="Q82" s="14">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="R82" s="24">
         <f>Q82</f>
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="S82" s="9"/>
       <c r="U82" s="7"/>
@@ -4654,11 +4722,11 @@
       </c>
       <c r="Q83" s="25">
         <f>Q82/2</f>
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="R83" s="14">
         <f>Q83</f>
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="S83" s="9"/>
       <c r="U83" s="7"/>
@@ -4682,11 +4750,11 @@
       </c>
       <c r="K84" s="25">
         <f>K82/2</f>
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="L84" s="14">
         <f>K84</f>
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="M84" s="9"/>
       <c r="N84" s="8"/>
@@ -4768,7 +4836,7 @@
         <v>11</v>
       </c>
       <c r="W86" s="16" t="e">
-        <f>apbp*W85/(W78*(1+W82/(W83+W87))/W80-1)</f>
+        <f>anbp*W85/(W78*(1+W82/(W83+W87))/W80-1)</f>
         <v>#N/A</v>
       </c>
       <c r="X86" s="14" t="e">
@@ -4793,12 +4861,12 @@
       <c r="V87" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="W87" s="26" t="e">
-        <f>apbp/(1/W83+1/W84)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X87" s="26" t="e">
-        <f>apbp/(1/X83+1/X84)</f>
+      <c r="W87" s="49" t="e">
+        <f>anbp/(1/W83+1/W84)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X87" s="49" t="e">
+        <f>anbp/(1/X83+1/X84)</f>
         <v>#N/A</v>
       </c>
       <c r="Y87" s="9"/>
@@ -4846,21 +4914,33 @@
       <c r="Y90" s="44"/>
     </row>
     <row r="91" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="I91" s="7"/>
+      <c r="I91" s="48" t="s">
+        <v>59</v>
+      </c>
       <c r="J91" s="8"/>
       <c r="K91" s="8"/>
       <c r="L91" s="8"/>
-      <c r="M91" s="9"/>
-      <c r="O91" s="7"/>
+      <c r="M91" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="O91" s="48" t="s">
+        <v>60</v>
+      </c>
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
       <c r="R91" s="8"/>
-      <c r="S91" s="9"/>
-      <c r="U91" s="7"/>
+      <c r="S91" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="U91" s="48" t="s">
+        <v>61</v>
+      </c>
       <c r="V91" s="8"/>
       <c r="W91" s="8"/>
       <c r="X91" s="8"/>
-      <c r="Y91" s="9"/>
+      <c r="Y91" s="46" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="92" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I92" s="7"/>
@@ -5138,7 +5218,7 @@
       </c>
       <c r="K105" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="L105" s="10" t="e">
         <f>L108*K103+L109</f>
@@ -5151,7 +5231,7 @@
       </c>
       <c r="Q105" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R105" s="10" t="e">
         <f>R108*Q103+R109</f>
@@ -5164,11 +5244,11 @@
       </c>
       <c r="W105" s="21">
         <f>Voutzs</f>
-        <v>-3</v>
-      </c>
-      <c r="X105" s="10" t="e">
+        <v>3</v>
+      </c>
+      <c r="X105" s="10">
         <f>X108*W103+X109</f>
-        <v>#N/A</v>
+        <v>3</v>
       </c>
       <c r="Y105" s="9"/>
     </row>
@@ -5179,7 +5259,7 @@
       </c>
       <c r="K106" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L106" s="10" t="e">
         <f>L108*K104+L109</f>
@@ -5192,7 +5272,7 @@
       </c>
       <c r="Q106" s="21">
         <f>Voutfs</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R106" s="10" t="e">
         <f>R108*Q104+R109</f>
@@ -5205,11 +5285,11 @@
       </c>
       <c r="W106" s="21">
         <f>Voutfs</f>
-        <v>1</v>
-      </c>
-      <c r="X106" s="10" t="e">
+        <v>-1</v>
+      </c>
+      <c r="X106" s="10">
         <f>X108*W104+X109</f>
-        <v>#N/A</v>
+        <v>-1</v>
       </c>
       <c r="Y106" s="9"/>
     </row>
@@ -5245,7 +5325,7 @@
       </c>
       <c r="K108" s="10">
         <f>(K106-K105)/(K104-K103)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="L108" s="10" t="e">
         <f>K110*(-L111/L112)</f>
@@ -5258,7 +5338,7 @@
       </c>
       <c r="Q108" s="10">
         <f>(Q106-Q105)/(Q104-Q103)</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R108" s="10" t="e">
         <f>Q110*(-R111/R112)</f>
@@ -5271,11 +5351,11 @@
       </c>
       <c r="W108" s="10">
         <f>(W106-W105)/(W104-W103)</f>
-        <v>2</v>
-      </c>
-      <c r="X108" s="23" t="e">
+        <v>-2</v>
+      </c>
+      <c r="X108" s="23">
         <f>-W110*X113/X114</f>
-        <v>#N/A</v>
+        <v>-2</v>
       </c>
       <c r="Y108" s="9"/>
     </row>
@@ -5286,7 +5366,7 @@
       </c>
       <c r="K109" s="10">
         <f>K105-K108*K103</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L109" s="10" t="e">
         <f>-K110*K107*L111/L113</f>
@@ -5299,7 +5379,7 @@
       </c>
       <c r="Q109" s="10">
         <f>Q105-Q108*Q103</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R109" s="10" t="e">
         <f>Q110*0</f>
@@ -5312,11 +5392,11 @@
       </c>
       <c r="W109" s="10">
         <f>W105-W108*W103</f>
-        <v>-1</v>
-      </c>
-      <c r="X109" s="23" t="e">
+        <v>1</v>
+      </c>
+      <c r="X109" s="23">
         <f>W110*X111*W107*(X113+X114)/(X114*(X111+X112))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="Y109" s="9"/>
     </row>
@@ -5345,9 +5425,9 @@
       <c r="V110" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W110" s="12" t="e">
+      <c r="W110" s="12">
         <f>IF(AND(W108&lt;=-1,W109&gt;0),1,NA())</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X110" s="12"/>
       <c r="Y110" s="9"/>
@@ -5381,13 +5461,13 @@
       <c r="V111" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="W111" s="13" t="e">
+      <c r="W111" s="13">
         <f>W110*W109*W112*W114/(W107*(W113+W114)-W109*W114)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X111" s="27" t="e">
+        <v>3357.1428571428573</v>
+      </c>
+      <c r="X111" s="27">
         <f>W111</f>
-        <v>#N/A</v>
+        <v>3357.1428571428573</v>
       </c>
       <c r="Y111" s="9"/>
     </row>
@@ -5400,8 +5480,9 @@
         <f>K110*K111/ABS(K108)</f>
         <v>#N/A</v>
       </c>
-      <c r="L112" s="27">
-        <v>15000</v>
+      <c r="L112" s="27" t="e">
+        <f>K112</f>
+        <v>#N/A</v>
       </c>
       <c r="M112" s="9"/>
       <c r="O112" s="7"/>
@@ -5476,13 +5557,13 @@
       <c r="V114" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="W114" s="16" t="e">
+      <c r="W114" s="16">
         <f>W110*W113/ABS(W108)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X114" s="27" t="e">
+        <v>11000</v>
+      </c>
+      <c r="X114" s="27">
         <f>W114</f>
-        <v>#N/A</v>
+        <v>11000</v>
       </c>
       <c r="Y114" s="9"/>
     </row>
@@ -5624,7 +5705,7 @@
       <formula>apbn=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{2FDBDC6C-E86F-458F-B9F2-A7D36482A9A8}">
       <formula1>$B$34:$B$45</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Rederived mpbn circuit and verified in LTSPice.
</commit_message>
<xml_diff>
--- a/OpAmp.xlsx
+++ b/OpAmp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\OpAmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3C9D4A-A534-4A9B-9C50-5D00C82F7C00}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F54A8A-907E-4425-BB4D-7F26289A70D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32835" windowHeight="15795" xr2:uid="{D6C93E9B-8E91-4E75-A6F3-2E8A3339D527}"/>
   </bookViews>
@@ -54,6 +54,21 @@
     <author>Marten Agren</author>
   </authors>
   <commentList>
+    <comment ref="K24" authorId="0" shapeId="0" xr:uid="{0B92AC02-57E9-44AC-847C-BEC26086C799}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Choose small relative to Rf &amp; Rg
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="Q24" authorId="0" shapeId="0" xr:uid="{94E5F1AF-4588-4B22-9F67-8F4613982D65}">
       <text>
         <r>
@@ -112,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K26" authorId="0" shapeId="0" xr:uid="{534AF19C-7992-4797-BB6B-0DE4F3F53713}">
+    <comment ref="K26" authorId="0" shapeId="0" xr:uid="{CDD8D1CB-9B70-468C-B662-8859FC299884}">
       <text>
         <r>
           <rPr>
@@ -122,7 +137,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Choose value (approx Rg/10)</t>
+          <t xml:space="preserve">Choose (perhaps suggested by datasheet)
+</t>
         </r>
       </text>
     </comment>
@@ -382,7 +398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="67">
   <si>
     <t>Vinfs</t>
   </si>
@@ -1081,50 +1097,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>228251</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>675821</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>56922</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A17174-B20A-476D-8BC9-E55351AE46CC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5657501" y="923924"/>
-          <a:ext cx="3495570" cy="1752373"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
@@ -1147,7 +1119,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1186,7 +1158,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1225,7 +1197,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1269,7 +1241,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1330,7 +1302,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1391,7 +1363,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1452,7 +1424,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1513,7 +1485,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1574,7 +1546,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1635,7 +1607,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1696,7 +1668,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1712,6 +1684,67 @@
         <a:xfrm>
           <a:off x="5895975" y="6934200"/>
           <a:ext cx="3383903" cy="1438275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13BCFF1F-B50B-46A0-BA52-C9E37290C56E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5629275" y="1009650"/>
+          <a:ext cx="3448050" cy="1781175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2032,7 +2065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978419D8-7C85-4718-8844-D6DF268777A2}">
   <dimension ref="B3:AE117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2098,8 +2133,8 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="47" t="s">
-        <v>65</v>
+      <c r="M4" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="48" t="s">
@@ -2283,7 +2318,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
@@ -2402,7 +2437,7 @@
       </c>
       <c r="C15" s="39">
         <f>VLOOKUP(C11,examples,4,)</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -2459,7 +2494,7 @@
       </c>
       <c r="C16" s="39">
         <f>VLOOKUP(C11,examples,5,)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -2556,7 +2591,7 @@
       </c>
       <c r="C18" s="34">
         <f>(C16-C15)/(C14-C13)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -2567,11 +2602,11 @@
       </c>
       <c r="K18" s="21">
         <f>Voutzs</f>
-        <v>3</v>
-      </c>
-      <c r="L18" s="10" t="e">
+        <v>-3</v>
+      </c>
+      <c r="L18" s="10">
         <f>L21*K16+L22</f>
-        <v>#N/A</v>
+        <v>-3</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="8"/>
@@ -2581,7 +2616,7 @@
       </c>
       <c r="Q18" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="R18" s="10" t="e">
         <f>R21*Q16+R22</f>
@@ -2594,7 +2629,7 @@
       </c>
       <c r="W18" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="X18" s="10" t="e">
         <f>X21*W16+X22</f>
@@ -2607,11 +2642,11 @@
       </c>
       <c r="AC18" s="21">
         <f>Voutzs</f>
-        <v>3</v>
-      </c>
-      <c r="AD18" s="10" t="e">
+        <v>-3</v>
+      </c>
+      <c r="AD18" s="10">
         <f>AD21*AC16+AD22</f>
-        <v>#N/A</v>
+        <v>-10.545454545454547</v>
       </c>
       <c r="AE18" s="9"/>
     </row>
@@ -2621,7 +2656,7 @@
       </c>
       <c r="C19" s="34">
         <f>C15-C18*C13</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E19" t="s">
         <v>39</v>
@@ -2633,11 +2668,11 @@
       </c>
       <c r="K19" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
-      </c>
-      <c r="L19" s="10" t="e">
+        <v>1</v>
+      </c>
+      <c r="L19" s="10">
         <f>L21*K17+L22</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="8"/>
@@ -2647,7 +2682,7 @@
       </c>
       <c r="Q19" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R19" s="10" t="e">
         <f>R21*Q17+R22</f>
@@ -2660,7 +2695,7 @@
       </c>
       <c r="W19" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X19" s="10" t="e">
         <f>X21*W17+X22</f>
@@ -2673,11 +2708,11 @@
       </c>
       <c r="AC19" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
-      </c>
-      <c r="AD19" s="10" t="e">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="10">
         <f>AD21*AC17+AD22</f>
-        <v>#N/A</v>
+        <v>0.54545454545454586</v>
       </c>
       <c r="AE19" s="9"/>
     </row>
@@ -2726,11 +2761,11 @@
       </c>
       <c r="K21" s="10">
         <f>(K19-K18)/(K17-K16)</f>
-        <v>-2</v>
-      </c>
-      <c r="L21" s="29" t="e">
-        <f>K23*(1+L25/L28)</f>
-        <v>#N/A</v>
+        <v>2</v>
+      </c>
+      <c r="L21" s="29">
+        <f>mpbn*(L26+L27+1/(1/L24+1/L25))/(L27+1/(1/L24+1/L25))</f>
+        <v>2</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="8"/>
@@ -2740,7 +2775,7 @@
       </c>
       <c r="Q21" s="10">
         <f>(Q19-Q18)/(Q17-Q16)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="R21" s="29" t="e">
         <f>Q23*IF(ISNUMBER(#REF!),(#REF!*R24/R25+#REF!)/(#REF!+#REF!),R24/R25+1)</f>
@@ -2753,7 +2788,7 @@
       </c>
       <c r="W21" s="10">
         <f>(W19-W18)/(W17-W16)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="X21" s="29" t="e">
         <f>W23*IF(ISNUMBER(X25),(X25*X26/X27+X25)/(X24+X25),X26/X27+1)</f>
@@ -2766,11 +2801,11 @@
       </c>
       <c r="AC21" s="10">
         <f>(AC19-AC18)/(AC17-AC16)</f>
-        <v>-2</v>
-      </c>
-      <c r="AD21" s="29" t="e">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="29">
         <f>AC23*(1+AD26/AD27)</f>
-        <v>#N/A</v>
+        <v>5.5454545454545459</v>
       </c>
       <c r="AE21" s="9"/>
     </row>
@@ -2781,11 +2816,11 @@
       </c>
       <c r="K22" s="10">
         <f>K18-K21*K16</f>
-        <v>1</v>
-      </c>
-      <c r="L22" s="29" t="e">
-        <f>-K23*L29*(L27+L25)/L27</f>
-        <v>#N/A</v>
+        <v>-1</v>
+      </c>
+      <c r="L22" s="29">
+        <f>-mpbn*K20*(L25/(L24+L25))*L26/(L27+1/(1/L24+1/L25))</f>
+        <v>-1</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="8"/>
@@ -2795,7 +2830,7 @@
       </c>
       <c r="Q22" s="10">
         <f>Q18-Q21*Q16</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R22" s="29" t="e">
         <f>Q23*0</f>
@@ -2808,7 +2843,7 @@
       </c>
       <c r="W22" s="10">
         <f>W18-W21*W16</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X22" s="29" t="e">
         <f>W23*IF(ISNUMBER(X25),W20*X24*X21/X25,0)</f>
@@ -2821,11 +2856,11 @@
       </c>
       <c r="AC22" s="10">
         <f>AC18-AC21*AC16</f>
-        <v>1</v>
-      </c>
-      <c r="AD22" s="29" t="e">
+        <v>-1</v>
+      </c>
+      <c r="AD22" s="29">
         <f>-AD21*AD28</f>
-        <v>#N/A</v>
+        <v>-5</v>
       </c>
       <c r="AE22" s="9"/>
     </row>
@@ -2843,9 +2878,9 @@
       <c r="J23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K23" s="12" t="e">
+      <c r="K23" s="12">
         <f>IF(AND(K21&gt;1,K22&lt;0),1,NA())</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="L23" s="12"/>
       <c r="M23" s="9"/>
@@ -2874,9 +2909,9 @@
       <c r="AB23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="12" t="e">
+      <c r="AC23" s="12">
         <f>IF(AND(AC21&gt;1,AC22&lt;0),1,NA())</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="AD23" s="12"/>
       <c r="AE23" s="9"/>
@@ -2890,13 +2925,12 @@
       <c r="J24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="24" t="e">
-        <f>K23*K26*(K20-K29)/K29</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L24" s="14" t="e">
+      <c r="K24" s="14">
+        <v>2200</v>
+      </c>
+      <c r="L24" s="14">
         <f>K24</f>
-        <v>#N/A</v>
+        <v>2200</v>
       </c>
       <c r="M24" s="9"/>
       <c r="N24" s="8"/>
@@ -2940,14 +2974,15 @@
     <row r="25" spans="2:31" x14ac:dyDescent="0.25">
       <c r="I25" s="7"/>
       <c r="J25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K25" s="14">
-        <v>22000</v>
+        <v>11</v>
+      </c>
+      <c r="K25" s="16">
+        <f>mpbn*K24/(K20*(1-K21)/K22-1)</f>
+        <v>550</v>
       </c>
       <c r="L25" s="24">
         <f>K25</f>
-        <v>22000</v>
+        <v>550</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="8"/>
@@ -2980,9 +3015,9 @@
       <c r="AB25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AC25" s="16" t="e">
+      <c r="AC25" s="16">
         <f>AC23*AC28*AC24/(AC20-AC28)</f>
-        <v>#N/A</v>
+        <v>1111.1111111111111</v>
       </c>
       <c r="AD25" s="14">
         <v>2200</v>
@@ -2992,15 +3027,14 @@
     <row r="26" spans="2:31" x14ac:dyDescent="0.25">
       <c r="I26" s="7"/>
       <c r="J26" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="25" t="e">
-        <f>K28/10</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L26" s="14" t="e">
+        <v>9</v>
+      </c>
+      <c r="K26" s="14">
+        <v>100000</v>
+      </c>
+      <c r="L26" s="14">
         <f>K26</f>
-        <v>#N/A</v>
+        <v>100000</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="8"/>
@@ -3036,15 +3070,15 @@
     <row r="27" spans="2:31" x14ac:dyDescent="0.25">
       <c r="I27" s="7"/>
       <c r="J27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K27" s="16" t="e">
-        <f>K28-K26</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L27" s="14" t="e">
+        <v>10</v>
+      </c>
+      <c r="K27" s="16">
+        <f>mpbn*K26/(K21-1)-1/(1/K24+1/K25)</f>
+        <v>99560</v>
+      </c>
+      <c r="L27" s="14">
         <f>K27</f>
-        <v>#N/A</v>
+        <v>99560</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="8"/>
@@ -3070,9 +3104,9 @@
       <c r="AB27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AC27" s="16" t="e">
+      <c r="AC27" s="16">
         <f>AC23*AC26/(AC21-1)</f>
-        <v>#N/A</v>
+        <v>10000</v>
       </c>
       <c r="AD27" s="14">
         <v>2200</v>
@@ -3081,17 +3115,9 @@
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.25">
       <c r="I28" s="7"/>
-      <c r="J28" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" s="26" t="e">
-        <f>K23*K25/(K21-1)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L28" s="26" t="e">
-        <f>L27+L26</f>
-        <v>#N/A</v>
-      </c>
+      <c r="J28" s="19"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
       <c r="M28" s="9"/>
       <c r="N28" s="8"/>
       <c r="O28" s="7"/>
@@ -3108,9 +3134,9 @@
       <c r="AB28" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AC28" s="30" t="e">
+      <c r="AC28" s="30">
         <f>AC23*ABS(AC22)/AC21</f>
-        <v>#N/A</v>
+        <v>0.5</v>
       </c>
       <c r="AD28" s="30">
         <f>AC20/(1+AD24/AD25)</f>
@@ -3120,17 +3146,9 @@
     </row>
     <row r="29" spans="2:31" x14ac:dyDescent="0.25">
       <c r="I29" s="7"/>
-      <c r="J29" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="30" t="e">
-        <f>K23*ABS(K22)*K27/(K27+K25)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L29" s="30" t="e">
-        <f>K20/(1+L24/L26)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="J29" s="19"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
       <c r="M29" s="9"/>
       <c r="N29" s="8"/>
       <c r="O29" s="7"/>
@@ -3696,7 +3714,7 @@
       </c>
       <c r="K47" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="L47" s="10" t="e">
         <f>L50*K45+L51</f>
@@ -3709,7 +3727,7 @@
       </c>
       <c r="Q47" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="R47" s="10" t="e">
         <f>R50*Q45+R51</f>
@@ -3722,7 +3740,7 @@
       </c>
       <c r="W47" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="X47" s="10" t="e">
         <f>X50*W45+X51</f>
@@ -3737,7 +3755,7 @@
       </c>
       <c r="K48" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L48" s="10" t="e">
         <f>L50*K46+L51</f>
@@ -3750,7 +3768,7 @@
       </c>
       <c r="Q48" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R48" s="10" t="e">
         <f>R50*Q46+R51</f>
@@ -3763,7 +3781,7 @@
       </c>
       <c r="W48" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X48" s="10" t="e">
         <f>X50*W46+X51</f>
@@ -3803,7 +3821,7 @@
       </c>
       <c r="K50" s="10">
         <f>(K48-K47)/(K46-K45)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="L50" s="10" t="e">
         <f>apbn*L54/(L53+L54)*(1+L55/L56)</f>
@@ -3816,7 +3834,7 @@
       </c>
       <c r="Q50" s="10">
         <f>(Q48-Q47)/(Q46-Q45)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="R50" s="10" t="e">
         <f>apbz*R54/(R53+R54)</f>
@@ -3829,7 +3847,7 @@
       </c>
       <c r="W50" s="10">
         <f>(W48-W47)/(W46-W45)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="X50" s="23" t="e">
         <f>(apbp/X53)/(1/X53+1/X54+1/X55)</f>
@@ -3845,7 +3863,7 @@
       </c>
       <c r="K51" s="10">
         <f>K47-K50*K45</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L51" s="10" t="e">
         <f>-apbn*K49*L55/L56</f>
@@ -3858,7 +3876,7 @@
       </c>
       <c r="Q51" s="10">
         <f>Q47-Q50*Q45</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R51" s="10" t="e">
         <f>Q52*0</f>
@@ -3871,7 +3889,7 @@
       </c>
       <c r="W51" s="10">
         <f>W47-W50*W45</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X51" s="23" t="e">
         <f>apbp*(W49/X55)/(1/X53+1/X54+1/X55)</f>
@@ -4442,7 +4460,7 @@
       </c>
       <c r="K76" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="L76" s="10" t="e">
         <f>L79*K74+L80</f>
@@ -4456,7 +4474,7 @@
       </c>
       <c r="Q76" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="R76" s="10" t="e">
         <f>R79*Q74+R80</f>
@@ -4469,7 +4487,7 @@
       </c>
       <c r="W76" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="X76" s="10" t="e">
         <f>X79*W74+X80</f>
@@ -4484,7 +4502,7 @@
       </c>
       <c r="K77" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L77" s="10" t="e">
         <f>L79*K75+L80</f>
@@ -4498,7 +4516,7 @@
       </c>
       <c r="Q77" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R77" s="10" t="e">
         <f>R79*Q75+R80</f>
@@ -4511,7 +4529,7 @@
       </c>
       <c r="W77" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X77" s="10" t="e">
         <f>X79*W75+X80</f>
@@ -4552,7 +4570,7 @@
       </c>
       <c r="K79" s="10">
         <f>(K77-K76)/(K75-K74)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="L79" s="29" t="e">
         <f>-apbn*IF(ISNUMBER(L85),L82*L85/(L84*(L84+2*L85)),1)</f>
@@ -4566,7 +4584,7 @@
       </c>
       <c r="Q79" s="10">
         <f>(Q77-Q76)/(Q75-Q74)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="R79" s="29" t="e">
         <f>-apbz*R82*R84/(R83*(R83+2*R84))</f>
@@ -4579,7 +4597,7 @@
       </c>
       <c r="W79" s="10">
         <f>(W77-W76)/(W75-W74)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="X79" s="29" t="e">
         <f>-anbp*X82*X84/(X83*(X83+2*X84))</f>
@@ -4594,7 +4612,7 @@
       </c>
       <c r="K80" s="10">
         <f>K76-K79*K74</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L80" s="10" t="e">
         <f>-K81*K78*L82/L83</f>
@@ -4608,7 +4626,7 @@
       </c>
       <c r="Q80" s="10">
         <f>Q76-Q79*Q74</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R80" s="29" t="e">
         <f>Q81*0</f>
@@ -4621,7 +4639,7 @@
       </c>
       <c r="W80" s="10">
         <f>W76-W79*W74</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X80" s="29" t="e">
         <f>anbp*W78*(X86/(X85+X86))*(1+X82/(X83+X87))</f>
@@ -5218,7 +5236,7 @@
       </c>
       <c r="K105" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="L105" s="10" t="e">
         <f>L108*K103+L109</f>
@@ -5231,7 +5249,7 @@
       </c>
       <c r="Q105" s="21">
         <f>Voutzs</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="R105" s="10" t="e">
         <f>R108*Q103+R109</f>
@@ -5244,11 +5262,11 @@
       </c>
       <c r="W105" s="21">
         <f>Voutzs</f>
-        <v>3</v>
-      </c>
-      <c r="X105" s="10">
+        <v>-3</v>
+      </c>
+      <c r="X105" s="10" t="e">
         <f>X108*W103+X109</f>
-        <v>3</v>
+        <v>#N/A</v>
       </c>
       <c r="Y105" s="9"/>
     </row>
@@ -5259,7 +5277,7 @@
       </c>
       <c r="K106" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L106" s="10" t="e">
         <f>L108*K104+L109</f>
@@ -5272,7 +5290,7 @@
       </c>
       <c r="Q106" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R106" s="10" t="e">
         <f>R108*Q104+R109</f>
@@ -5285,11 +5303,11 @@
       </c>
       <c r="W106" s="21">
         <f>Voutfs</f>
-        <v>-1</v>
-      </c>
-      <c r="X106" s="10">
+        <v>1</v>
+      </c>
+      <c r="X106" s="10" t="e">
         <f>X108*W104+X109</f>
-        <v>-1</v>
+        <v>#N/A</v>
       </c>
       <c r="Y106" s="9"/>
     </row>
@@ -5325,7 +5343,7 @@
       </c>
       <c r="K108" s="10">
         <f>(K106-K105)/(K104-K103)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="L108" s="10" t="e">
         <f>K110*(-L111/L112)</f>
@@ -5338,7 +5356,7 @@
       </c>
       <c r="Q108" s="10">
         <f>(Q106-Q105)/(Q104-Q103)</f>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="R108" s="10" t="e">
         <f>Q110*(-R111/R112)</f>
@@ -5351,11 +5369,11 @@
       </c>
       <c r="W108" s="10">
         <f>(W106-W105)/(W104-W103)</f>
-        <v>-2</v>
-      </c>
-      <c r="X108" s="23">
+        <v>2</v>
+      </c>
+      <c r="X108" s="23" t="e">
         <f>-W110*X113/X114</f>
-        <v>-2</v>
+        <v>#N/A</v>
       </c>
       <c r="Y108" s="9"/>
     </row>
@@ -5366,7 +5384,7 @@
       </c>
       <c r="K109" s="10">
         <f>K105-K108*K103</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L109" s="10" t="e">
         <f>-K110*K107*L111/L113</f>
@@ -5379,7 +5397,7 @@
       </c>
       <c r="Q109" s="10">
         <f>Q105-Q108*Q103</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R109" s="10" t="e">
         <f>Q110*0</f>
@@ -5392,11 +5410,11 @@
       </c>
       <c r="W109" s="10">
         <f>W105-W108*W103</f>
-        <v>1</v>
-      </c>
-      <c r="X109" s="23">
+        <v>-1</v>
+      </c>
+      <c r="X109" s="23" t="e">
         <f>W110*X111*W107*(X113+X114)/(X114*(X111+X112))</f>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="Y109" s="9"/>
     </row>
@@ -5425,9 +5443,9 @@
       <c r="V110" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W110" s="12">
+      <c r="W110" s="12" t="e">
         <f>IF(AND(W108&lt;=-1,W109&gt;0),1,NA())</f>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="X110" s="12"/>
       <c r="Y110" s="9"/>
@@ -5461,13 +5479,13 @@
       <c r="V111" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="W111" s="13">
+      <c r="W111" s="13" t="e">
         <f>W110*W109*W112*W114/(W107*(W113+W114)-W109*W114)</f>
-        <v>3357.1428571428573</v>
-      </c>
-      <c r="X111" s="27">
+        <v>#N/A</v>
+      </c>
+      <c r="X111" s="27" t="e">
         <f>W111</f>
-        <v>3357.1428571428573</v>
+        <v>#N/A</v>
       </c>
       <c r="Y111" s="9"/>
     </row>
@@ -5557,13 +5575,13 @@
       <c r="V114" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="W114" s="16">
+      <c r="W114" s="16" t="e">
         <f>W110*W113/ABS(W108)</f>
-        <v>11000</v>
-      </c>
-      <c r="X114" s="27">
+        <v>#N/A</v>
+      </c>
+      <c r="X114" s="27" t="e">
         <f>W114</f>
-        <v>11000</v>
+        <v>#N/A</v>
       </c>
       <c r="Y114" s="9"/>
     </row>

</xml_diff>

<commit_message>
Corrected derivation of mpbne case.
</commit_message>
<xml_diff>
--- a/OpAmp.xlsx
+++ b/OpAmp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\OpAmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F54A8A-907E-4425-BB4D-7F26289A70D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F9C2DE-4486-42FB-89EE-4B9C654E4989}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32835" windowHeight="15795" xr2:uid="{D6C93E9B-8E91-4E75-A6F3-2E8A3339D527}"/>
   </bookViews>
@@ -398,7 +398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="66">
   <si>
     <t>Vinfs</t>
   </si>
@@ -593,9 +593,6 @@
   </si>
   <si>
     <t>mpbne</t>
-  </si>
-  <si>
-    <t>unverified</t>
   </si>
   <si>
     <t>Verson 1.1, 20180609, Marten Agren</t>
@@ -612,7 +609,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,13 +700,6 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -817,7 +807,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -919,7 +909,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2065,9 +2054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978419D8-7C85-4718-8844-D6DF268777A2}">
   <dimension ref="B3:AE117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2125,9 +2112,9 @@
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="47" t="s">
         <v>50</v>
       </c>
       <c r="J4" s="8"/>
@@ -2137,7 +2124,7 @@
         <v>63</v>
       </c>
       <c r="N4" s="8"/>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="47" t="s">
         <v>51</v>
       </c>
       <c r="P4" s="8"/>
@@ -2146,7 +2133,7 @@
       <c r="S4" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="U4" s="48" t="s">
+      <c r="U4" s="47" t="s">
         <v>55</v>
       </c>
       <c r="V4" s="8"/>
@@ -2155,14 +2142,14 @@
       <c r="Y4" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="AA4" s="48" t="s">
+      <c r="AA4" s="47" t="s">
         <v>64</v>
       </c>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
-      <c r="AE4" s="47" t="s">
-        <v>65</v>
+      <c r="AE4" s="46" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
@@ -3017,7 +3004,7 @@
       </c>
       <c r="AC25" s="16">
         <f>AC23*AC28*AC24/(AC20-AC28)</f>
-        <v>1111.1111111111111</v>
+        <v>2500</v>
       </c>
       <c r="AD25" s="14">
         <v>2200</v>
@@ -3135,8 +3122,8 @@
         <v>16</v>
       </c>
       <c r="AC28" s="30">
-        <f>AC23*ABS(AC22)/AC21</f>
-        <v>0.5</v>
+        <f>AC23*ABS(AC22)/(AC21-1)</f>
+        <v>1</v>
       </c>
       <c r="AD28" s="30">
         <f>AC20/(1+AD24/AD25)</f>
@@ -3230,7 +3217,7 @@
       <c r="F33" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I33" s="48" t="s">
+      <c r="I33" s="47" t="s">
         <v>52</v>
       </c>
       <c r="J33" s="8"/>
@@ -3239,7 +3226,7 @@
       <c r="M33" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="O33" s="48" t="s">
+      <c r="O33" s="47" t="s">
         <v>53</v>
       </c>
       <c r="P33" s="8"/>
@@ -3248,7 +3235,7 @@
       <c r="S33" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="U33" s="48" t="s">
+      <c r="U33" s="47" t="s">
         <v>54</v>
       </c>
       <c r="V33" s="8"/>
@@ -4142,7 +4129,7 @@
       <c r="Y61" s="44"/>
     </row>
     <row r="62" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="I62" s="48" t="s">
+      <c r="I62" s="47" t="s">
         <v>56</v>
       </c>
       <c r="J62" s="8"/>
@@ -4152,7 +4139,7 @@
         <v>63</v>
       </c>
       <c r="N62" s="8"/>
-      <c r="O62" s="48" t="s">
+      <c r="O62" s="47" t="s">
         <v>57</v>
       </c>
       <c r="P62" s="8"/>
@@ -4161,7 +4148,7 @@
       <c r="S62" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="U62" s="48" t="s">
+      <c r="U62" s="47" t="s">
         <v>58</v>
       </c>
       <c r="V62" s="8"/>
@@ -4879,11 +4866,11 @@
       <c r="V87" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="W87" s="49" t="e">
+      <c r="W87" s="48" t="e">
         <f>anbp/(1/W83+1/W84)</f>
         <v>#N/A</v>
       </c>
-      <c r="X87" s="49" t="e">
+      <c r="X87" s="48" t="e">
         <f>anbp/(1/X83+1/X84)</f>
         <v>#N/A</v>
       </c>
@@ -4932,7 +4919,7 @@
       <c r="Y90" s="44"/>
     </row>
     <row r="91" spans="9:25" x14ac:dyDescent="0.25">
-      <c r="I91" s="48" t="s">
+      <c r="I91" s="47" t="s">
         <v>59</v>
       </c>
       <c r="J91" s="8"/>
@@ -4941,7 +4928,7 @@
       <c r="M91" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="O91" s="48" t="s">
+      <c r="O91" s="47" t="s">
         <v>60</v>
       </c>
       <c r="P91" s="8"/>
@@ -4950,7 +4937,7 @@
       <c r="S91" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="U91" s="48" t="s">
+      <c r="U91" s="47" t="s">
         <v>61</v>
       </c>
       <c r="V91" s="8"/>
@@ -5723,7 +5710,7 @@
       <formula>apbn=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{2FDBDC6C-E86F-458F-B9F2-A7D36482A9A8}">
       <formula1>$B$34:$B$45</formula1>
     </dataValidation>

</xml_diff>